<commit_message>
Upates to rGC tree and Thermotaxis Worm Tracker
</commit_message>
<xml_diff>
--- a/Code/Plotting in R/Data/Adaptation_R_Import.xlsx
+++ b/Code/Plotting in R/Data/Adaptation_R_Import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Box Sync/Lab_Hallem/Astra/Writing/Bryant et al 20xx/Data/Calcium Imaging/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Documents/RStudio/Bryant_et_al_2021/Code/Plotting in R/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C7044E-3664-A94A-B710-2D078DCB5948}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495A6391-9CB2-4645-BE26-7EF0F75CE352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="3220" windowWidth="32740" windowHeight="16440" xr2:uid="{3004599B-148A-194A-83D2-70A6D74987AA}"/>
+    <workbookView xWindow="16000" yWindow="2040" windowWidth="32740" windowHeight="16440" xr2:uid="{3004599B-148A-194A-83D2-70A6D74987AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="126">
   <si>
     <t>Ss</t>
   </si>
@@ -352,13 +352,64 @@
   </si>
   <si>
     <t>210416_006</t>
+  </si>
+  <si>
+    <t>FlincG3</t>
+  </si>
+  <si>
+    <t>211014_004</t>
+  </si>
+  <si>
+    <t>211014_005</t>
+  </si>
+  <si>
+    <t>211014_006</t>
+  </si>
+  <si>
+    <t>211014_007</t>
+  </si>
+  <si>
+    <t>211014_008</t>
+  </si>
+  <si>
+    <t>211014_009</t>
+  </si>
+  <si>
+    <t>211014_010</t>
+  </si>
+  <si>
+    <t>211105_001</t>
+  </si>
+  <si>
+    <t>211105_002</t>
+  </si>
+  <si>
+    <t>211105_003</t>
+  </si>
+  <si>
+    <t>211105_004</t>
+  </si>
+  <si>
+    <t>211105_005</t>
+  </si>
+  <si>
+    <t>211105_006</t>
+  </si>
+  <si>
+    <t>211105_007</t>
+  </si>
+  <si>
+    <t>211105_008</t>
+  </si>
+  <si>
+    <t>211105_009</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -387,6 +438,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -408,12 +472,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,16 +793,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5911F61E-9712-514B-8E64-67B2F8452371}">
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:H112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J80" sqref="J80"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F116" sqref="F116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -3230,13 +3296,430 @@
         <v>12</v>
       </c>
       <c r="G96" s="3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H96" s="2" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>-33.403019009584341</v>
+      </c>
+      <c r="B97">
+        <v>-28.390682987433959</v>
+      </c>
+      <c r="C97">
+        <v>-1</v>
+      </c>
+      <c r="D97">
+        <v>-1</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G97" s="5">
+        <v>23</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>-35.663218001864379</v>
+      </c>
+      <c r="B98">
+        <v>-30.062769656673396</v>
+      </c>
+      <c r="C98">
+        <v>-1</v>
+      </c>
+      <c r="D98">
+        <v>-1</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G98" s="5">
+        <v>23</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>-34.758773229374469</v>
+      </c>
+      <c r="B99">
+        <v>-27.022726481926693</v>
+      </c>
+      <c r="C99">
+        <v>-1</v>
+      </c>
+      <c r="D99">
+        <v>-1</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G99" s="5">
+        <v>23</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>-23.520502860350376</v>
+      </c>
+      <c r="B100">
+        <v>-18.995014886184251</v>
+      </c>
+      <c r="C100">
+        <v>-1</v>
+      </c>
+      <c r="D100">
+        <v>-1</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G100" s="5">
+        <v>23</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>-38.166158900474933</v>
+      </c>
+      <c r="B101">
+        <v>-35.810948142667556</v>
+      </c>
+      <c r="C101">
+        <v>-1</v>
+      </c>
+      <c r="D101">
+        <v>-1</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G101" s="5">
+        <v>23</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>-43.77940844748975</v>
+      </c>
+      <c r="B102">
+        <v>-42.558776095686781</v>
+      </c>
+      <c r="C102">
+        <v>-1</v>
+      </c>
+      <c r="D102">
+        <v>-1</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G102" s="5">
+        <v>23</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>-40.565457054816036</v>
+      </c>
+      <c r="B103">
+        <v>-36.720240987508824</v>
+      </c>
+      <c r="C103">
+        <v>-1</v>
+      </c>
+      <c r="D103">
+        <v>-1</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G103" s="5">
+        <v>23</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>-26.647719439484842</v>
+      </c>
+      <c r="B104">
+        <v>-18.773374140069368</v>
+      </c>
+      <c r="C104">
+        <v>-1</v>
+      </c>
+      <c r="D104">
+        <v>-1</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G104" s="5">
+        <v>23</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>-27.177539336590534</v>
+      </c>
+      <c r="B105">
+        <v>-21.720950490749242</v>
+      </c>
+      <c r="C105">
+        <v>-1</v>
+      </c>
+      <c r="D105">
+        <v>-1</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G105" s="5">
+        <v>23</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>-24.714028928373562</v>
+      </c>
+      <c r="B106">
+        <v>-20.702107948759764</v>
+      </c>
+      <c r="C106">
+        <v>-1</v>
+      </c>
+      <c r="D106">
+        <v>-1</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G106" s="5">
+        <v>23</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>-21.794911837769671</v>
+      </c>
+      <c r="B107">
+        <v>-15.008172247681792</v>
+      </c>
+      <c r="C107">
+        <v>-1</v>
+      </c>
+      <c r="D107">
+        <v>-1</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G107" s="5">
+        <v>23</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>-20.048273995614956</v>
+      </c>
+      <c r="B108">
+        <v>-16.70657169897531</v>
+      </c>
+      <c r="C108">
+        <v>-1</v>
+      </c>
+      <c r="D108">
+        <v>-1</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G108" s="5">
+        <v>23</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>-35.363888752349453</v>
+      </c>
+      <c r="B109">
+        <v>-24.01738185433825</v>
+      </c>
+      <c r="C109">
+        <v>-1</v>
+      </c>
+      <c r="D109">
+        <v>-1</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G109" s="5">
+        <v>23</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>-29.431318670980716</v>
+      </c>
+      <c r="B110">
+        <v>-21.287664147896407</v>
+      </c>
+      <c r="C110">
+        <v>-1</v>
+      </c>
+      <c r="D110">
+        <v>-1</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G110" s="5">
+        <v>23</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>-17.775888963715381</v>
+      </c>
+      <c r="B111">
+        <v>-10.30252262034193</v>
+      </c>
+      <c r="C111">
+        <v>-1</v>
+      </c>
+      <c r="D111">
+        <v>-1</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G111" s="5">
+        <v>23</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>-24.6912942040723</v>
+      </c>
+      <c r="B112">
+        <v>-15.368392939912667</v>
+      </c>
+      <c r="C112">
+        <v>-1</v>
+      </c>
+      <c r="D112">
+        <v>-1</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G112" s="5">
+        <v>23</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating imaging code and results
</commit_message>
<xml_diff>
--- a/Code/Plotting in R/Data/Adaptation_R_Import.xlsx
+++ b/Code/Plotting in R/Data/Adaptation_R_Import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Documents/RStudio/Bryant_et_al_2021/Code/Plotting in R/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC6C144-220B-684D-9B21-2FDAAE305999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E582E62-96AE-F54A-8E49-71786E3FE397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="4020" windowWidth="32740" windowHeight="16440" xr2:uid="{3004599B-148A-194A-83D2-70A6D74987AA}"/>
   </bookViews>
@@ -695,8 +695,8 @@
   <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67:D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,7 +737,7 @@
         <v>1.4871201115106227</v>
       </c>
       <c r="B2">
-        <v>9.1346612853952518</v>
+        <v>9.9457514024314158</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -760,10 +760,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>-16.767250134868171</v>
+        <v>-16.22779182725651</v>
       </c>
       <c r="B3">
-        <v>11.174559700225087</v>
+        <v>12.872114284246949</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -786,10 +786,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>-20.128209138978576</v>
+        <v>-18.762619497260452</v>
       </c>
       <c r="B4">
-        <v>3.3812181981136886</v>
+        <v>-5.1938099456774731E-2</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -812,10 +812,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>-20.789239631360694</v>
+        <v>-19.213902499303479</v>
       </c>
       <c r="B5">
-        <v>3.4041995798102116</v>
+        <v>1.6215566659970464</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -838,10 +838,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>-13.097951466359845</v>
+        <v>-11.477784012965978</v>
       </c>
       <c r="B6">
-        <v>5.0614343132066404</v>
+        <v>5.3253362240968904</v>
       </c>
       <c r="C6">
         <v>-1</v>
@@ -864,10 +864,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>-17.160435076977393</v>
+        <v>-16.712062265707708</v>
       </c>
       <c r="B7">
-        <v>4.9700001256384398</v>
+        <v>6.7620619070295112</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -890,10 +890,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>29.198934919395512</v>
+        <v>17.398772667603374</v>
       </c>
       <c r="B8">
-        <v>12.395791675436389</v>
+        <v>12.665775030016647</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -916,13 +916,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>-7.6652062410309103</v>
+        <v>-8.1211474688400553</v>
       </c>
       <c r="B9">
-        <v>4.3676204287713878</v>
+        <v>1.721637871511049</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -942,10 +942,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>-17.365520250760813</v>
+        <v>-14.019244026089597</v>
       </c>
       <c r="B10">
-        <v>-2.8106820473863934</v>
+        <v>-2.2027669800954284</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -968,16 +968,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>-11.745448559048198</v>
+        <v>-10.126233970702842</v>
       </c>
       <c r="B11">
-        <v>6.414505340755932</v>
+        <v>9.0914208275220822</v>
       </c>
       <c r="C11">
         <v>-1</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>0</v>
@@ -994,10 +994,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>8.643364246399198</v>
+        <v>7.1366443546039591</v>
       </c>
       <c r="B12">
-        <v>6.2802540986513922</v>
+        <v>4.7560909738728592</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1020,10 +1020,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>-22.800720144234482</v>
+        <v>-21.529648906424708</v>
       </c>
       <c r="B13">
-        <v>-0.20773490776299869</v>
+        <v>2.7339900409015634E-2</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -1046,10 +1046,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>-26.625918958422389</v>
+        <v>-24.861478598620529</v>
       </c>
       <c r="B14">
-        <v>-2.2240309636392044</v>
+        <v>-0.27924864813734385</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -1072,10 +1072,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>-20.094194473489594</v>
+        <v>-13.731266704883502</v>
       </c>
       <c r="B15">
-        <v>-3.3896777994995166</v>
+        <v>-3.5918967031508751</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>-9.942906235428012</v>
+        <v>-8.086671755685007</v>
       </c>
       <c r="B16">
-        <v>1.414096738345914</v>
+        <v>-0.92779311623438798</v>
       </c>
       <c r="C16">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1124,10 +1124,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>-12.086820515453647</v>
+        <v>-7.688470137958757</v>
       </c>
       <c r="B17">
-        <v>2.3239039522709364</v>
+        <v>-1.8418377904994645</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -1150,10 +1150,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>-25.396454541736379</v>
+        <v>-24.327347629743567</v>
       </c>
       <c r="B18">
-        <v>-5.7152983995932169</v>
+        <v>-6.7529538521736017</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -1176,10 +1176,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>-4.9638698331746509</v>
+        <v>-3.8104606250983761</v>
       </c>
       <c r="B19">
-        <v>11.691343581370802</v>
+        <v>12.581720944013441</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1202,13 +1202,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>4.2063685993831692</v>
+        <v>6.0840805446344719</v>
       </c>
       <c r="B20">
-        <v>8.6221373031128721</v>
+        <v>8.9854813352036764</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1228,10 +1228,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>17.726427358626239</v>
+        <v>13.252201117910749</v>
       </c>
       <c r="B21">
-        <v>15.336654017628927</v>
+        <v>17.344856514968459</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1254,10 +1254,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>-6.1381733902761582</v>
+        <v>-3.372349111463377</v>
       </c>
       <c r="B22">
-        <v>2.9778411311712887</v>
+        <v>2.625542137375044</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1280,10 +1280,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>2.6200384262495406</v>
+        <v>4.8480038015272848</v>
       </c>
       <c r="B23">
-        <v>11.034395324538146</v>
+        <v>10.597007347183315</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1306,10 +1306,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>-7.5768332373631875</v>
+        <v>-6.4292273870743779</v>
       </c>
       <c r="B24">
-        <v>2.7295058808064079</v>
+        <v>3.2047844443032618</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1332,10 +1332,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>-12.02488095923332</v>
+        <v>-11.711013854029947</v>
       </c>
       <c r="B25">
-        <v>-6.0749119129143931</v>
+        <v>-5.4303223761000243</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -1358,10 +1358,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>-6.2672933295514897</v>
+        <v>-5.3934835600455315</v>
       </c>
       <c r="B26">
-        <v>4.330843131569095</v>
+        <v>5.0086905956888206</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1384,10 +1384,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>-7.5200317004024742</v>
+        <v>-7.1560825487814883</v>
       </c>
       <c r="B27">
-        <v>3.2343208088117841</v>
+        <v>3.4796470349906397</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1410,10 +1410,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>-5.3309651895815788</v>
+        <v>-4.4291851525713142</v>
       </c>
       <c r="B28">
-        <v>7.2319403259357449</v>
+        <v>7.2829315716837817</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1436,10 +1436,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>-4.8235369881232106</v>
+        <v>-2.4475031420629643</v>
       </c>
       <c r="B29">
-        <v>8.4744071784484376</v>
+        <v>8.0613314205745734</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>-13.353363724277651</v>
+        <v>-10.873827969576475</v>
       </c>
       <c r="B30">
         <v>-3.3844144581927509</v>
@@ -1488,13 +1488,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>-0.43509032898248101</v>
+        <v>0.15864049147768533</v>
       </c>
       <c r="B31">
-        <v>11.059451640685392</v>
+        <v>11.764910001832355</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1514,10 +1514,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>-10.434200374848945</v>
+        <v>-9.2299935727186195</v>
       </c>
       <c r="B32">
-        <v>2.0971918745869611</v>
+        <v>3.3264225571310422</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1540,10 +1540,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>2.6137381680931613</v>
+        <v>2.6501186201025959</v>
       </c>
       <c r="B33">
-        <v>12.7180224491464</v>
+        <v>12.794730333956959</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1566,10 +1566,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>-2.2740668914552487</v>
+        <v>-0.97112141811364827</v>
       </c>
       <c r="B34">
-        <v>7.0629838848725681</v>
+        <v>7.2734026462298997</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1592,10 +1592,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>14.337800972964644</v>
+        <v>12.131513351561036</v>
       </c>
       <c r="B35">
-        <v>7.1430610639125094</v>
+        <v>6.560894496417772</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1621,7 +1621,7 @@
         <v>12.95166123130273</v>
       </c>
       <c r="B36">
-        <v>12.582726969205337</v>
+        <v>12.776229815279043</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1644,10 +1644,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>24.484074095571781</v>
+        <v>24.109819821928571</v>
       </c>
       <c r="B37">
-        <v>22.101494258146356</v>
+        <v>21.04196456646984</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1670,10 +1670,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>11.873242863254891</v>
+        <v>12.892348505638003</v>
       </c>
       <c r="B38">
-        <v>17.39949057212382</v>
+        <v>18.058104480505275</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1696,10 +1696,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>11.763841426388471</v>
+        <v>15.212012006084837</v>
       </c>
       <c r="B39">
-        <v>18.655118949590758</v>
+        <v>19.642951521202328</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1722,10 +1722,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>5.8401133763168342</v>
+        <v>6.3153491417835195</v>
       </c>
       <c r="B40">
-        <v>6.8251949451447604</v>
+        <v>7.4714656539394202</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1748,10 +1748,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>10.898791872017986</v>
+        <v>12.692016854258048</v>
       </c>
       <c r="B41">
-        <v>17.471737014422814</v>
+        <v>15.006505167144956</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1774,10 +1774,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>12.895821657573684</v>
+        <v>14.044924372030614</v>
       </c>
       <c r="B42">
-        <v>18.714258901666938</v>
+        <v>19.075535212858135</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -1800,10 +1800,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>21.730695305752704</v>
+        <v>20.656866475143282</v>
       </c>
       <c r="B43">
-        <v>23.832325713874091</v>
+        <v>24.896528581236694</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1826,10 +1826,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>13.129234210171973</v>
+        <v>13.222956540584669</v>
       </c>
       <c r="B44">
-        <v>18.565832889193508</v>
+        <v>19.239993606155767</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -1855,7 +1855,7 @@
         <v>22.600381425861013</v>
       </c>
       <c r="B45">
-        <v>21.745710360291184</v>
+        <v>22.365475125576808</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -1878,10 +1878,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>24.835197670560369</v>
+        <v>25.722624399712306</v>
       </c>
       <c r="B46">
-        <v>30.763889167248504</v>
+        <v>31.655256810818724</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1904,10 +1904,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>15.041371277343561</v>
+        <v>15.62119021778031</v>
       </c>
       <c r="B47">
-        <v>17.883743891977783</v>
+        <v>17.562304141326678</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1930,10 +1930,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>21.633607715140322</v>
+        <v>20.290157242676521</v>
       </c>
       <c r="B48">
-        <v>16.67466103884486</v>
+        <v>17.353504072624254</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -1956,7 +1956,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>16.386367713515316</v>
+        <v>16.077147891735581</v>
       </c>
       <c r="B49">
         <v>17.720325916298258</v>
@@ -1982,10 +1982,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>22.704586588386086</v>
+        <v>22.799589176657165</v>
       </c>
       <c r="B50">
-        <v>23.138941959404121</v>
+        <v>22.599613662957012</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -2008,10 +2008,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>5.5217119770092964</v>
+        <v>6.4082551977968301</v>
       </c>
       <c r="B51">
-        <v>9.1366836359408357</v>
+        <v>9.3294471828599423</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -2034,10 +2034,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>-24.843719940466798</v>
+        <v>-24.873135113216243</v>
       </c>
       <c r="B52">
-        <v>-25.488381378798941</v>
+        <v>-25.755349079564191</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2060,10 +2060,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>-25.177205474734706</v>
+        <v>-24.875083265084267</v>
       </c>
       <c r="B53">
-        <v>-26.099274576159239</v>
+        <v>-24.409758526275617</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2086,10 +2086,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>-37.437415839483549</v>
+        <v>-37.544353187634499</v>
       </c>
       <c r="B54">
-        <v>-40.53415440178496</v>
+        <v>-40.684975259707841</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -2112,10 +2112,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>-10.854184802638246</v>
+        <v>-10.778018334986911</v>
       </c>
       <c r="B55">
-        <v>-11.617950900760436</v>
+        <v>-11.454154094149816</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -2138,10 +2138,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>-10.762064891468135</v>
+        <v>-11.136454681680419</v>
       </c>
       <c r="B56">
-        <v>-10.294110369215215</v>
+        <v>-10.262091694722585</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -2164,10 +2164,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>-18.121056618773437</v>
+        <v>-17.765383152890397</v>
       </c>
       <c r="B57">
-        <v>-17.736529964113313</v>
+        <v>-17.720475352420188</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -2190,10 +2190,10 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>-31.817506315350553</v>
+        <v>-30.792502924531966</v>
       </c>
       <c r="B58">
-        <v>-35.895148161916751</v>
+        <v>-36.145824948859996</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -2216,10 +2216,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>-12.002138584917143</v>
+        <v>-12.511234904713865</v>
       </c>
       <c r="B59">
-        <v>-14.967032968199735</v>
+        <v>-14.946722086268622</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -2242,10 +2242,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>-8.4392822084105603</v>
+        <v>-8.9853182332310997</v>
       </c>
       <c r="B60">
-        <v>-8.859624365515991</v>
+        <v>-8.8869956869158813</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -2268,13 +2268,13 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>-23.90069787709723</v>
+        <v>-21.398317412547868</v>
       </c>
       <c r="B61">
-        <v>-25.353706108083607</v>
+        <v>-25.118466490239317</v>
       </c>
       <c r="C61">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D61">
         <v>-1</v>
@@ -2294,7 +2294,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>-24.770671647441816</v>
+        <v>-24.873746951706174</v>
       </c>
       <c r="B62">
         <v>-26.716395606617162</v>
@@ -2320,10 +2320,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>-25.552336135450737</v>
+        <v>-24.902638210545732</v>
       </c>
       <c r="B63">
-        <v>-23.946068905697071</v>
+        <v>-26.397074514756589</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -2346,10 +2346,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>-19.076468332228963</v>
+        <v>-18.86208241199752</v>
       </c>
       <c r="B64">
-        <v>-19.091214068369485</v>
+        <v>-18.881073905738333</v>
       </c>
       <c r="C64">
         <v>-1</v>
@@ -2372,10 +2372,10 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>-14.86587328981525</v>
+        <v>-13.509683055749477</v>
       </c>
       <c r="B65">
-        <v>-14.774406943598372</v>
+        <v>-13.939138596374963</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -2398,10 +2398,10 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>-24.636142829540944</v>
+        <v>-23.706394564714799</v>
       </c>
       <c r="B66">
-        <v>-25.40071736476586</v>
+        <v>-25.736659939356962</v>
       </c>
       <c r="C66">
         <v>-1</v>
@@ -2424,10 +2424,10 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>-33.195561090407054</v>
+        <v>-33.118021758364293</v>
       </c>
       <c r="B67">
-        <v>-27.880409090485326</v>
+        <v>-27.973104672777847</v>
       </c>
       <c r="C67">
         <v>-1</v>
@@ -2450,10 +2450,10 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>-35.508615854874435</v>
+        <v>-34.99258303305264</v>
       </c>
       <c r="B68">
-        <v>-28.464260788439923</v>
+        <v>-27.42414430317514</v>
       </c>
       <c r="C68">
         <v>-1</v>
@@ -2476,10 +2476,10 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>-34.03412582863605</v>
+        <v>-33.963113678167957</v>
       </c>
       <c r="B69">
-        <v>-26.297126538625488</v>
+        <v>-25.050919946027729</v>
       </c>
       <c r="C69">
         <v>-1</v>
@@ -2502,10 +2502,10 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>-23.468277345187225</v>
+        <v>-22.904701527763415</v>
       </c>
       <c r="B70">
-        <v>-18.364960683738033</v>
+        <v>-17.921402496864111</v>
       </c>
       <c r="C70">
         <v>-1</v>
@@ -2528,10 +2528,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>-38.174655734847775</v>
+        <v>-37.848725049947952</v>
       </c>
       <c r="B71">
-        <v>-35.652635055225318</v>
+        <v>-35.613090562840448</v>
       </c>
       <c r="C71">
         <v>-1</v>
@@ -2554,10 +2554,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>-43.623957487518716</v>
+        <v>-43.154281196093386</v>
       </c>
       <c r="B72">
-        <v>-42.582286529440651</v>
+        <v>-42.711110919854995</v>
       </c>
       <c r="C72">
         <v>-1</v>
@@ -2580,10 +2580,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>-40.617763508346108</v>
+        <v>-40.424150088831986</v>
       </c>
       <c r="B73">
-        <v>-35.76259513199571</v>
+        <v>-35.495343115765799</v>
       </c>
       <c r="C73">
         <v>-1</v>
@@ -2606,10 +2606,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>-26.70204361280582</v>
+        <v>-26.50770118653357</v>
       </c>
       <c r="B74">
-        <v>-18.368918611717469</v>
+        <v>-17.706431315247762</v>
       </c>
       <c r="C74">
         <v>-1</v>
@@ -2632,10 +2632,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>-26.772026500811457</v>
+        <v>-25.678959939580214</v>
       </c>
       <c r="B75">
-        <v>-21.308069547205339</v>
+        <v>-22.332681922100271</v>
       </c>
       <c r="C75">
         <v>-1</v>
@@ -2658,10 +2658,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>-24.870622576452607</v>
+        <v>-24.701195170738917</v>
       </c>
       <c r="B76">
-        <v>-19.922192890494959</v>
+        <v>-17.750409923852693</v>
       </c>
       <c r="C76">
         <v>-1</v>
@@ -2684,10 +2684,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>-21.353960825104817</v>
+        <v>-20.919435762154773</v>
       </c>
       <c r="B77">
-        <v>-14.994839684412458</v>
+        <v>-14.709197735329703</v>
       </c>
       <c r="C77">
         <v>-1</v>
@@ -2710,10 +2710,10 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>-19.925819391552373</v>
+        <v>-19.599885212518146</v>
       </c>
       <c r="B78">
-        <v>-16.70657169897531</v>
+        <v>-16.485362718893704</v>
       </c>
       <c r="C78">
         <v>-1</v>
@@ -2736,10 +2736,10 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>-35.26053294299949</v>
+        <v>-34.086871540602985</v>
       </c>
       <c r="B79">
-        <v>-22.232473397558813</v>
+        <v>-23.866553450233123</v>
       </c>
       <c r="C79">
         <v>-1</v>
@@ -2762,10 +2762,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>-29.497514908850121</v>
+        <v>-29.038292927411526</v>
       </c>
       <c r="B80">
-        <v>-20.660365610498456</v>
+        <v>-18.864035407723804</v>
       </c>
       <c r="C80">
         <v>-1</v>
@@ -2788,10 +2788,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>-18.31081234492251</v>
+        <v>-18.060895945245818</v>
       </c>
       <c r="B81">
-        <v>-8.8882230467969112</v>
+        <v>-5.0938708355221838</v>
       </c>
       <c r="C81">
         <v>-1</v>
@@ -2814,10 +2814,10 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>-24.666300410985649</v>
+        <v>-24.504368395250665</v>
       </c>
       <c r="B82">
-        <v>-15.190764094337602</v>
+        <v>-15.09641347107663</v>
       </c>
       <c r="C82">
         <v>-1</v>

</xml_diff>